<commit_message>
test: make update_files check xval and explain output. update test outputs for xval, and some files for explain
</commit_message>
<xml_diff>
--- a/tests/data/experiments/lr-xval-xlsx/output/evaluation/output/lr_xval_xlsx_evaluation_test_excluded_composition.xlsx
+++ b/tests/data/experiments/lr-xval-xlsx/output/evaluation/output/lr_xval_xlsx_evaluation_test_excluded_composition.xlsx
@@ -446,11 +446,7 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
+      <c r="A2" t="inlineStr"/>
       <c r="B2" t="n">
         <v>0</v>
       </c>

</xml_diff>